<commit_message>
Added row to list all characters for easy reference during data entry
</commit_message>
<xml_diff>
--- a/StoryBreakdown.xlsx
+++ b/StoryBreakdown.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="179">
   <si>
     <t xml:space="preserve">Title</t>
   </si>
@@ -660,6 +660,9 @@
   </si>
   <si>
     <t xml:space="preserve">XXXIw2. Married hero loses his wife, resumed marriage as result of quest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dramatis Personae</t>
   </si>
 </sst>
 </file>
@@ -849,10 +852,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A178"/>
+  <dimension ref="A1:A180"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A151" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A173" activeCellId="0" sqref="A173:A178"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A184" activeCellId="0" sqref="A184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65"/>
@@ -1749,6 +1752,11 @@
     <row r="178" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="1" t="s">
         <v>177</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="0" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -1770,7 +1778,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A173:A178 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1799,7 +1807,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A173:A178 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>